<commit_message>
update ip to 192.168.1.x
</commit_message>
<xml_diff>
--- a/VM_list.xlsx
+++ b/VM_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22098" windowHeight="9222"/>
+    <workbookView windowWidth="21000" windowHeight="7902"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
     <t>catpc</t>
   </si>
   <si>
-    <t>192.168.121.100</t>
+    <t>192.168.1.99</t>
   </si>
   <si>
     <t>Origin Ubuntu</t>
@@ -65,7 +65,7 @@
     <t>k8smaster</t>
   </si>
   <si>
-    <t>192.168.121.111</t>
+    <t>192.168.1.111</t>
   </si>
   <si>
     <t xml:space="preserve">K8s master </t>
@@ -74,7 +74,7 @@
     <t>k8sworker1</t>
   </si>
   <si>
-    <t>192.168.121.112</t>
+    <t>192.168.1.112</t>
   </si>
   <si>
     <t>K8s worker 1</t>
@@ -83,7 +83,7 @@
     <t>k8sworker2</t>
   </si>
   <si>
-    <t>192.168.121.113</t>
+    <t>192.168.1.113</t>
   </si>
   <si>
     <t>K8s worker 2</t>
@@ -92,7 +92,7 @@
     <t>rancherserver</t>
   </si>
   <si>
-    <t>192.168.121.114</t>
+    <t>192.168.1.114</t>
   </si>
   <si>
     <t>rancher.devopsedu.vn</t>
@@ -107,7 +107,7 @@
     <t>loadbalance</t>
   </si>
   <si>
-    <t>192.168.121.99</t>
+    <t>192.168.1.100</t>
   </si>
   <si>
     <t>Load Balance</t>
@@ -1353,7 +1353,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8859649122807" defaultRowHeight="14.4" outlineLevelCol="7"/>

</xml_diff>